<commit_message>
refactor: compare_to_expected_result function + more import_csv_file tests
</commit_message>
<xml_diff>
--- a/tests/integration/inputs/import_csv_file/test.xlsx
+++ b/tests/integration/inputs/import_csv_file/test.xlsx
@@ -29,9 +29,9 @@
       <text>
         <r>
           <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -41,13 +41,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -57,13 +57,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -73,13 +73,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -89,13 +89,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -105,13 +105,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -121,13 +121,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="H1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -137,13 +137,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="I1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -154,13 +154,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="J1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -170,13 +170,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="K1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -186,13 +186,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="L1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -202,13 +202,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="M1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -220,13 +220,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="N1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -238,13 +238,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="O1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -255,13 +255,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="P1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -272,13 +272,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="Q1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -288,13 +288,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="R1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -307,13 +307,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="S1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -326,13 +326,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="T1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -343,13 +343,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="U1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -360,13 +360,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="V1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -376,13 +376,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="W1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -393,13 +393,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="X1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -410,13 +410,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="Y1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -428,13 +428,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="Z1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -446,13 +446,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AA1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -463,13 +463,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AB1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -478,13 +478,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AC1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -496,13 +496,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AD1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -513,13 +513,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AE1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -529,13 +529,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AF1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -547,13 +547,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AG1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -563,13 +563,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AH1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -579,13 +579,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AI1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -595,13 +595,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AJ1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -611,13 +611,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AK1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -627,13 +627,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AL1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -643,13 +643,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AL1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AM1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -659,13 +659,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AN1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -675,13 +675,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AO1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -691,13 +691,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AP1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -707,13 +707,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AQ1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -723,13 +723,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AR1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -739,13 +739,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AR1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AS1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -755,13 +755,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AT1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -772,13 +772,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AU1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -789,13 +789,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AV1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -804,13 +804,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AW1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -819,13 +819,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AX1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -834,13 +834,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AX1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AY1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -849,13 +849,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AY1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AZ1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -864,13 +864,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AZ1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="BA1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -879,13 +879,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="BA1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="BB1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -894,13 +894,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="BB1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="BC1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -909,13 +909,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="BC1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="BD1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -924,13 +924,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="BD1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="BE1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -940,13 +940,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="BE1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="BF1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -956,13 +956,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="BF1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="BG1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -972,13 +972,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="BG1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="BH1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -988,13 +988,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="BH1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="BI1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -1004,13 +1004,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="BI1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="BJ1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -1025,11 +1025,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="110">
   <si>
     <t xml:space="preserve">Code-barres</t>
   </si>
   <si>
+    <t xml:space="preserve">Organisation</t>
+  </si>
+  <si>
     <t xml:space="preserve">Identifiant produit du producteur</t>
   </si>
   <si>
@@ -1298,6 +1301,60 @@
   </si>
   <si>
     <t xml:space="preserve">https://my-server.com/images/lentils-1.jpg, https://my-server.com/images/lentils-2.jpg </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Food Company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peaches</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Etats-Unis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White peaches, high fructose corn syrup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">World Test Food</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Super bananes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bananes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5 kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">World Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Martinique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Banane</t>
   </si>
 </sst>
 </file>
@@ -1307,7 +1364,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1335,13 +1392,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -1511,87 +1561,87 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BI2"/>
+  <dimension ref="A1:BJ4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BC1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BC3" activeCellId="0" sqref="BC3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="8" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="55.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="25.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="17" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="24.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="36.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="24.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="43.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="41.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="27" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="21.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="32.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="34.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="46.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="39.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="28.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="26.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="39.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="29.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="23.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="41" style="0" width="26.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="75.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="52.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="45" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="26.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="49" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="0" width="35.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="0" width="32.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="0" width="62.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="0" width="37.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="0" width="46.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="0" width="42.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="0" width="80.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="0" width="36.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="61" style="0" width="27.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="33.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="9" style="0" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="55.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="25.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="18" style="0" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="24.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="36.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="24.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="43.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="41.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="28" style="0" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="21.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="31" style="0" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="32.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="34.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="46.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="39.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="28.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="26.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="39.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="29.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="23.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="42" style="0" width="26.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="75.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="52.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="46" style="0" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="26.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="50" style="0" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="0" width="35.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="0" width="32.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="0" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="0" width="62.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="0" width="37.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="0" width="46.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="0" width="42.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="0" width="80.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="61" style="0" width="36.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="62" style="0" width="27.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -1600,34 +1650,34 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
       <c r="V1" s="3" t="s">
@@ -1636,22 +1686,22 @@
       <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="3" t="s">
         <v>25</v>
       </c>
       <c r="AA1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AB1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="3" t="s">
         <v>28</v>
       </c>
       <c r="AD1" s="1" t="s">
@@ -1687,19 +1737,19 @@
       <c r="AN1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AO1" s="1" t="s">
         <v>40</v>
       </c>
       <c r="AP1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>42</v>
       </c>
       <c r="AR1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AS1" s="1" t="s">
         <v>44</v>
       </c>
       <c r="AT1" s="2" t="s">
@@ -1720,19 +1770,19 @@
       <c r="AY1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="3" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>51</v>
       </c>
       <c r="BA1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BB1" s="3" t="s">
         <v>53</v>
       </c>
       <c r="BC1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BD1" s="2" t="s">
         <v>55</v>
       </c>
       <c r="BE1" s="1" t="s">
@@ -1744,25 +1794,25 @@
       <c r="BG1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="BH1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BI1" s="2" t="s">
         <v>60</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>3270190128403</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="0" t="n">
         <v>34</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>62</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>63</v>
@@ -1776,13 +1826,13 @@
       <c r="H2" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>66</v>
+      <c r="I2" s="0" t="s">
+        <v>67</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="L2" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>67</v>
       </c>
       <c r="M2" s="0" t="s">
@@ -1807,34 +1857,34 @@
         <v>74</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="W2" s="0" t="s">
         <v>75</v>
       </c>
+      <c r="U2" s="0" t="s">
+        <v>72</v>
+      </c>
       <c r="X2" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z2" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="AB2" s="0" t="s">
+      <c r="Y2" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA2" s="0" t="s">
         <v>77</v>
       </c>
       <c r="AC2" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="AE2" s="0" t="s">
+      <c r="AD2" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="AF2" s="0" t="n">
+      <c r="AF2" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="AG2" s="0" t="n">
         <v>1409</v>
       </c>
-      <c r="AG2" s="0" t="n">
+      <c r="AH2" s="0" t="n">
         <v>333</v>
-      </c>
-      <c r="AH2" s="0" t="s">
-        <v>80</v>
       </c>
       <c r="AI2" s="0" t="s">
         <v>81</v>
@@ -1857,23 +1907,108 @@
       <c r="AO2" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="AU2" s="0" t="n">
+      <c r="AP2" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="AV2" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="BC2" s="0" t="s">
-        <v>88</v>
       </c>
       <c r="BD2" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="BH2" s="0" t="s">
+      <c r="BE2" s="0" t="s">
         <v>90</v>
+      </c>
+      <c r="BI2" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>4270190128403</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="T3" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD3" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="AG3" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="AI3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ3" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK3" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="AL3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="AM3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AO3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU3" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>5270190128403</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y4" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="AD4" s="0" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="BC2" r:id="rId2" display="https://www.carrefour.fr/p/lentilles-bio-vertes-carrefour-bio-3270190128403"/>
-    <hyperlink ref="BD2" r:id="rId3" display="http://my-server.com/images/lentils.jpg"/>
+    <hyperlink ref="BD2" r:id="rId2" display="https://www.carrefour.fr/p/lentilles-bio-vertes-carrefour-bio-3270190128403"/>
+    <hyperlink ref="BE2" r:id="rId3" display="http://my-server.com/images/lentils.jpg"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
refactor: compare_to_expected_result function + more import_csv_file tests (#7168)
* refactor: compare_to_expected_result function + more import_csv_file tests

* refactor: compare_to_expected_result function + more import_csv_file tests
</commit_message>
<xml_diff>
--- a/tests/integration/inputs/import_csv_file/test.xlsx
+++ b/tests/integration/inputs/import_csv_file/test.xlsx
@@ -29,9 +29,9 @@
       <text>
         <r>
           <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -41,13 +41,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -57,13 +57,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -73,13 +73,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -89,13 +89,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -105,13 +105,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -121,13 +121,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="H1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -137,13 +137,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="I1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -154,13 +154,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="J1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -170,13 +170,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="K1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -186,13 +186,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="L1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -202,13 +202,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="M1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -220,13 +220,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="N1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -238,13 +238,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="O1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -255,13 +255,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="P1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -272,13 +272,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="Q1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -288,13 +288,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="R1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -307,13 +307,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="S1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -326,13 +326,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="T1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -343,13 +343,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="U1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -360,13 +360,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="V1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -376,13 +376,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="W1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -393,13 +393,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="X1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -410,13 +410,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="Y1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -428,13 +428,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="Z1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -446,13 +446,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AA1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -463,13 +463,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AB1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -478,13 +478,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AC1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -496,13 +496,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AD1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -513,13 +513,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AE1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -529,13 +529,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AF1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -547,13 +547,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AG1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -563,13 +563,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AH1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -579,13 +579,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AI1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -595,13 +595,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AJ1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -611,13 +611,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AK1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -627,13 +627,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AL1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -643,13 +643,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AL1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AM1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -659,13 +659,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AN1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -675,13 +675,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AO1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -691,13 +691,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AP1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -707,13 +707,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AQ1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -723,13 +723,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AR1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -739,13 +739,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AR1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AS1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -755,13 +755,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AT1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -772,13 +772,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AT1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AU1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -789,13 +789,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AV1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -804,13 +804,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AW1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -819,13 +819,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AX1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -834,13 +834,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AX1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AY1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -849,13 +849,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AY1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="AZ1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -864,13 +864,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="AZ1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="BA1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -879,13 +879,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="BA1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="BB1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -894,13 +894,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="BB1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="BC1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -909,13 +909,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="BC1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="BD1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -924,13 +924,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="BD1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="BE1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -940,13 +940,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="BE1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="BF1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -956,13 +956,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="BF1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="BG1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -972,13 +972,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="BG1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="BH1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -988,13 +988,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="BH1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="BI1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -1004,13 +1004,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="BI1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+    <comment ref="BJ1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -1025,11 +1025,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="110">
   <si>
     <t xml:space="preserve">Code-barres</t>
   </si>
   <si>
+    <t xml:space="preserve">Organisation</t>
+  </si>
+  <si>
     <t xml:space="preserve">Identifiant produit du producteur</t>
   </si>
   <si>
@@ -1298,6 +1301,60 @@
   </si>
   <si>
     <t xml:space="preserve">https://my-server.com/images/lentils-1.jpg, https://my-server.com/images/lentils-2.jpg </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Food Company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peaches</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Etats-Unis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White peaches, high fructose corn syrup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">World Test Food</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Super bananes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bananes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5 kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">World Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Martinique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Banane</t>
   </si>
 </sst>
 </file>
@@ -1307,7 +1364,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1335,13 +1392,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -1511,87 +1561,87 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BI2"/>
+  <dimension ref="A1:BJ4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BC1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BC3" activeCellId="0" sqref="BC3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="8" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="55.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="25.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="17" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="24.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="36.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="24.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="43.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="41.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="27" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="21.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="32.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="34.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="46.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="39.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="28.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="26.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="39.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="29.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="23.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="41" style="0" width="26.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="75.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="52.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="45" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="26.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="49" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="0" width="35.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="0" width="32.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="0" width="62.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="0" width="37.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="0" width="46.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="0" width="42.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="0" width="80.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="0" width="36.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="61" style="0" width="27.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="33.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="9" style="0" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="55.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="25.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="18" style="0" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="24.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="36.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="24.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="43.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="41.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="28" style="0" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="21.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="31" style="0" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="32.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="34.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="46.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="39.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="28.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="26.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="39.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="29.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="23.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="42" style="0" width="26.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="75.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="52.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="46" style="0" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="26.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="50" style="0" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="0" width="35.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="0" width="32.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="0" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="0" width="62.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="0" width="37.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="0" width="46.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="0" width="42.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="0" width="80.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="61" style="0" width="36.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="62" style="0" width="27.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -1600,34 +1650,34 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
       <c r="V1" s="3" t="s">
@@ -1636,22 +1686,22 @@
       <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="3" t="s">
         <v>25</v>
       </c>
       <c r="AA1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AB1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="3" t="s">
         <v>28</v>
       </c>
       <c r="AD1" s="1" t="s">
@@ -1687,19 +1737,19 @@
       <c r="AN1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AO1" s="1" t="s">
         <v>40</v>
       </c>
       <c r="AP1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>42</v>
       </c>
       <c r="AR1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AS1" s="1" t="s">
         <v>44</v>
       </c>
       <c r="AT1" s="2" t="s">
@@ -1720,19 +1770,19 @@
       <c r="AY1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="3" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>51</v>
       </c>
       <c r="BA1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BB1" s="3" t="s">
         <v>53</v>
       </c>
       <c r="BC1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BD1" s="2" t="s">
         <v>55</v>
       </c>
       <c r="BE1" s="1" t="s">
@@ -1744,25 +1794,25 @@
       <c r="BG1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="BH1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BI1" s="2" t="s">
         <v>60</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>3270190128403</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="0" t="n">
         <v>34</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>62</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>63</v>
@@ -1776,13 +1826,13 @@
       <c r="H2" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>66</v>
+      <c r="I2" s="0" t="s">
+        <v>67</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="L2" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>67</v>
       </c>
       <c r="M2" s="0" t="s">
@@ -1807,34 +1857,34 @@
         <v>74</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="W2" s="0" t="s">
         <v>75</v>
       </c>
+      <c r="U2" s="0" t="s">
+        <v>72</v>
+      </c>
       <c r="X2" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z2" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="AB2" s="0" t="s">
+      <c r="Y2" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA2" s="0" t="s">
         <v>77</v>
       </c>
       <c r="AC2" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="AE2" s="0" t="s">
+      <c r="AD2" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="AF2" s="0" t="n">
+      <c r="AF2" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="AG2" s="0" t="n">
         <v>1409</v>
       </c>
-      <c r="AG2" s="0" t="n">
+      <c r="AH2" s="0" t="n">
         <v>333</v>
-      </c>
-      <c r="AH2" s="0" t="s">
-        <v>80</v>
       </c>
       <c r="AI2" s="0" t="s">
         <v>81</v>
@@ -1857,23 +1907,108 @@
       <c r="AO2" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="AU2" s="0" t="n">
+      <c r="AP2" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="AV2" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="BC2" s="0" t="s">
-        <v>88</v>
       </c>
       <c r="BD2" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="BH2" s="0" t="s">
+      <c r="BE2" s="0" t="s">
         <v>90</v>
+      </c>
+      <c r="BI2" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>4270190128403</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="T3" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD3" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="AG3" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="AI3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ3" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK3" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="AL3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="AM3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AO3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU3" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>5270190128403</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y4" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="AD4" s="0" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="BC2" r:id="rId2" display="https://www.carrefour.fr/p/lentilles-bio-vertes-carrefour-bio-3270190128403"/>
-    <hyperlink ref="BD2" r:id="rId3" display="http://my-server.com/images/lentils.jpg"/>
+    <hyperlink ref="BD2" r:id="rId2" display="https://www.carrefour.fr/p/lentilles-bio-vertes-carrefour-bio-3270190128403"/>
+    <hyperlink ref="BE2" r:id="rId3" display="http://my-server.com/images/lentils.jpg"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
fix: changes needed for Lactalis Fromages import through Agena3000 (#7401)
* orgs with a gln but no party name
</commit_message>
<xml_diff>
--- a/tests/integration/inputs/import_csv_file/test.xlsx
+++ b/tests/integration/inputs/import_csv_file/test.xlsx
@@ -1025,7 +1025,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="112">
   <si>
     <t xml:space="preserve">Code-barres</t>
   </si>
@@ -1213,6 +1213,9 @@
     <t xml:space="preserve">Type de la photo du produit</t>
   </si>
   <si>
+    <t xml:space="preserve">Carrefour</t>
+  </si>
+  <si>
     <t xml:space="preserve">xb22-a33</t>
   </si>
   <si>
@@ -1243,9 +1246,6 @@
     <t xml:space="preserve">Carrefour Bio, Carrefour</t>
   </si>
   <si>
-    <t xml:space="preserve">Carrefour</t>
-  </si>
-  <si>
     <t xml:space="preserve">Plant-based foods and beverages, Plant-based foods, Legumes and their products, Cereals and potatoes, Fruits and vegetables based foods, Legumes, Seeds, Legume seeds, Vegetables based foods, Pulses, Lentils, Green lentils</t>
   </si>
   <si>
@@ -1355,6 +1355,12 @@
   </si>
   <si>
     <t xml:space="preserve">Banane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some product without an org name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some product</t>
   </si>
 </sst>
 </file>
@@ -1561,13 +1567,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BJ4"/>
+  <dimension ref="A1:BJ5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="33.71"/>
@@ -1808,47 +1814,50 @@
       <c r="A2" s="0" t="n">
         <v>3270190128403</v>
       </c>
+      <c r="B2" s="0" t="s">
+        <v>62</v>
+      </c>
       <c r="C2" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>34</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="R2" s="0" t="s">
         <v>73</v>
@@ -1860,7 +1869,7 @@
         <v>75</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="X2" s="0" t="s">
         <v>76</v>
@@ -1984,7 +1993,7 @@
         <v>103</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>104</v>
@@ -2003,6 +2012,17 @@
       </c>
       <c r="AD4" s="0" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>6270190128403</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>